<commit_message>
update design add productDetail Header products update Cart login
</commit_message>
<xml_diff>
--- a/design/chitiet/Cart.xlsx
+++ b/design/chitiet/Cart.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="117">
   <si>
     <t xml:space="preserve">Posts and Telecommunications Institute of Technology
 </t>
@@ -536,6 +536,24 @@
     <t xml:space="preserve">1. Thực hiện khởi tạo màn hình ban đầu</t>
   </si>
   <si>
+    <t xml:space="preserve">a. Check hạng mục</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nội dung check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user chưa login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chuyển trang login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“empty_token_err”</t>
+  </si>
+  <si>
     <t xml:space="preserve">(2) Xử lý xóa sản phẩm </t>
   </si>
   <si>
@@ -557,7 +575,7 @@
     <numFmt numFmtId="168" formatCode="yyyy\年m\月d\日;@"/>
     <numFmt numFmtId="169" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -669,8 +687,17 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="9"/>
+      <color rgb="FF660E7A"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,8 +728,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1053,6 +1086,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="hair"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1091,7 +1131,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="199">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1756,13 +1796,137 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="19" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="42" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="32" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="32" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="47" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="47" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="48" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="48" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="49" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="50" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1776,6 +1940,66 @@
     <cellStyle name="標準_基本要件仕様書_20061109" xfId="21"/>
     <cellStyle name="標準_基本設計書(FWIH105)" xfId="22"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660E7A"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1790,9 +2014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>35640</xdr:colOff>
+      <xdr:colOff>35280</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1806,7 +2030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3453840" y="22755240"/>
-          <a:ext cx="675000" cy="969120"/>
+          <a:ext cx="674640" cy="968760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1827,9 +2051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>155520</xdr:colOff>
+      <xdr:colOff>155160</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1839,7 +2063,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2177280" y="24338880"/>
-          <a:ext cx="955080" cy="645120"/>
+          <a:ext cx="954720" cy="644760"/>
         </a:xfrm>
         <a:prstGeom prst="can">
           <a:avLst>
@@ -1894,13 +2118,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>163800</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>69120</xdr:colOff>
+      <xdr:colOff>68760</xdr:colOff>
       <xdr:row>136</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1909,8 +2133,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2582640" y="23725800"/>
-          <a:ext cx="1207440" cy="617760"/>
+          <a:off x="2582640" y="23725080"/>
+          <a:ext cx="1207080" cy="617400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1955,9 +2179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>121320</xdr:colOff>
+      <xdr:colOff>120960</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1967,7 +2191,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2365920" y="22507560"/>
-          <a:ext cx="2778840" cy="2607480"/>
+          <a:ext cx="2778480" cy="2607120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1999,9 +2223,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>73800</xdr:colOff>
+      <xdr:colOff>73440</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2011,7 +2235,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3165480" y="22231440"/>
-          <a:ext cx="1187640" cy="426240"/>
+          <a:ext cx="1187280" cy="425880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2069,9 +2293,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>64080</xdr:colOff>
+      <xdr:colOff>63720</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2081,7 +2305,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="372240" y="23184000"/>
-          <a:ext cx="994320" cy="397440"/>
+          <a:ext cx="993960" cy="397080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2243,9 +2467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>178200</xdr:colOff>
+      <xdr:colOff>177840</xdr:colOff>
       <xdr:row>135</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2255,7 +2479,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6335280" y="23621760"/>
-          <a:ext cx="912960" cy="397800"/>
+          <a:ext cx="912600" cy="397440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2311,9 +2535,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>83160</xdr:colOff>
+      <xdr:colOff>82800</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2327,7 +2551,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6478200" y="22755240"/>
-          <a:ext cx="675000" cy="969120"/>
+          <a:ext cx="674640" cy="968760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2342,15 +2566,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>84600</xdr:colOff>
+      <xdr:colOff>84240</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>30600</xdr:colOff>
+      <xdr:colOff>29880</xdr:colOff>
       <xdr:row>136</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2359,8 +2583,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3805560" y="23691240"/>
-          <a:ext cx="1248480" cy="578880"/>
+          <a:off x="3804840" y="23690520"/>
+          <a:ext cx="1248120" cy="578520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2405,9 +2629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>167400</xdr:colOff>
+      <xdr:colOff>167040</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2417,7 +2641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4608000" y="24268680"/>
-          <a:ext cx="955080" cy="645120"/>
+          <a:ext cx="954720" cy="644760"/>
         </a:xfrm>
         <a:prstGeom prst="can">
           <a:avLst>
@@ -2476,9 +2700,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>26640</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2488,7 +2712,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3351240" y="24373800"/>
-          <a:ext cx="955080" cy="645120"/>
+          <a:ext cx="954720" cy="644760"/>
         </a:xfrm>
         <a:prstGeom prst="can">
           <a:avLst>
@@ -2543,13 +2767,13 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>20520</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>51480</xdr:colOff>
+      <xdr:colOff>51120</xdr:colOff>
       <xdr:row>137</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2558,8 +2782,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3741480" y="23745600"/>
-          <a:ext cx="30960" cy="685440"/>
+          <a:off x="3741480" y="23744880"/>
+          <a:ext cx="30600" cy="685080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2609,9 +2833,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2621,7 +2845,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1788840" y="1451880"/>
-          <a:ext cx="4816080" cy="416520"/>
+          <a:ext cx="4815720" cy="416160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2657,9 +2881,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>82440</xdr:colOff>
+      <xdr:colOff>82080</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2673,7 +2897,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="186120" y="1038240"/>
-          <a:ext cx="8730360" cy="5398560"/>
+          <a:ext cx="8730000" cy="5398200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2695,7 +2919,7 @@
   </sheetPr>
   <dimension ref="A1:AX160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E149" activeCellId="0" sqref="E149"/>
     </sheetView>
   </sheetViews>
@@ -10601,10 +10825,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ183"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A123" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C163" activeCellId="0" sqref="C163"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC156" activeCellId="0" sqref="AC156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16682,49 +16906,51 @@
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="17"/>
-      <c r="C156" s="0"/>
-      <c r="D156" s="0"/>
-      <c r="E156" s="0"/>
-      <c r="F156" s="0"/>
-      <c r="G156" s="0"/>
-      <c r="H156" s="0"/>
-      <c r="I156" s="0"/>
-      <c r="J156" s="0"/>
-      <c r="K156" s="0"/>
-      <c r="L156" s="0"/>
-      <c r="M156" s="0"/>
-      <c r="N156" s="0"/>
-      <c r="O156" s="0"/>
-      <c r="P156" s="0"/>
-      <c r="Q156" s="0"/>
-      <c r="R156" s="0"/>
-      <c r="S156" s="0"/>
-      <c r="T156" s="0"/>
-      <c r="U156" s="0"/>
-      <c r="V156" s="0"/>
-      <c r="W156" s="0"/>
-      <c r="X156" s="0"/>
-      <c r="Y156" s="0"/>
-      <c r="Z156" s="0"/>
-      <c r="AA156" s="0"/>
-      <c r="AB156" s="0"/>
-      <c r="AC156" s="0"/>
-      <c r="AD156" s="0"/>
-      <c r="AE156" s="0"/>
-      <c r="AF156" s="0"/>
-      <c r="AG156" s="0"/>
-      <c r="AH156" s="0"/>
-      <c r="AI156" s="0"/>
-      <c r="AJ156" s="0"/>
-      <c r="AK156" s="0"/>
-      <c r="AL156" s="0"/>
-      <c r="AM156" s="0"/>
-      <c r="AN156" s="0"/>
-      <c r="AO156" s="0"/>
-      <c r="AP156" s="0"/>
-      <c r="AQ156" s="0"/>
-      <c r="AR156" s="0"/>
-      <c r="AS156" s="0"/>
+      <c r="C156" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="D156" s="19"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="19"/>
+      <c r="G156" s="19"/>
+      <c r="H156" s="19"/>
+      <c r="I156" s="19"/>
+      <c r="J156" s="19"/>
+      <c r="K156" s="19"/>
+      <c r="L156" s="19"/>
+      <c r="M156" s="19"/>
+      <c r="N156" s="19"/>
+      <c r="O156" s="19"/>
+      <c r="P156" s="19"/>
+      <c r="Q156" s="19"/>
+      <c r="R156" s="19"/>
+      <c r="S156" s="19"/>
+      <c r="T156" s="19"/>
+      <c r="U156" s="19"/>
+      <c r="V156" s="19"/>
+      <c r="W156" s="19"/>
+      <c r="X156" s="19"/>
+      <c r="Y156" s="19"/>
+      <c r="Z156" s="19"/>
+      <c r="AA156" s="19"/>
+      <c r="AB156" s="19"/>
+      <c r="AC156" s="1"/>
+      <c r="AD156" s="19"/>
+      <c r="AE156" s="19"/>
+      <c r="AF156" s="19"/>
+      <c r="AG156" s="19"/>
+      <c r="AH156" s="19"/>
+      <c r="AI156" s="19"/>
+      <c r="AJ156" s="19"/>
+      <c r="AK156" s="19"/>
+      <c r="AL156" s="19"/>
+      <c r="AM156" s="19"/>
+      <c r="AN156" s="19"/>
+      <c r="AO156" s="19"/>
+      <c r="AP156" s="19"/>
+      <c r="AQ156" s="19"/>
+      <c r="AR156" s="19"/>
+      <c r="AS156" s="19"/>
       <c r="AT156" s="0"/>
       <c r="AU156" s="0"/>
       <c r="AV156" s="0"/>
@@ -16745,49 +16971,57 @@
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="17"/>
-      <c r="C157" s="0"/>
-      <c r="D157" s="0"/>
-      <c r="E157" s="0"/>
-      <c r="F157" s="0"/>
-      <c r="G157" s="0"/>
-      <c r="H157" s="0"/>
-      <c r="I157" s="0"/>
-      <c r="J157" s="0"/>
-      <c r="K157" s="0"/>
-      <c r="L157" s="0"/>
-      <c r="M157" s="0"/>
-      <c r="N157" s="0"/>
-      <c r="O157" s="0"/>
-      <c r="P157" s="0"/>
-      <c r="Q157" s="0"/>
-      <c r="R157" s="0"/>
-      <c r="S157" s="0"/>
-      <c r="T157" s="0"/>
-      <c r="U157" s="0"/>
-      <c r="V157" s="0"/>
-      <c r="W157" s="0"/>
-      <c r="X157" s="0"/>
-      <c r="Y157" s="0"/>
-      <c r="Z157" s="0"/>
-      <c r="AA157" s="0"/>
-      <c r="AB157" s="0"/>
-      <c r="AC157" s="0"/>
-      <c r="AD157" s="0"/>
-      <c r="AE157" s="0"/>
-      <c r="AF157" s="0"/>
-      <c r="AG157" s="0"/>
-      <c r="AH157" s="0"/>
-      <c r="AI157" s="0"/>
-      <c r="AJ157" s="0"/>
-      <c r="AK157" s="0"/>
-      <c r="AL157" s="0"/>
-      <c r="AM157" s="0"/>
-      <c r="AN157" s="0"/>
-      <c r="AO157" s="0"/>
-      <c r="AP157" s="0"/>
-      <c r="AQ157" s="0"/>
-      <c r="AR157" s="0"/>
-      <c r="AS157" s="0"/>
+      <c r="C157" s="166" t="s">
+        <v>49</v>
+      </c>
+      <c r="D157" s="167" t="s">
+        <v>68</v>
+      </c>
+      <c r="E157" s="167"/>
+      <c r="F157" s="167"/>
+      <c r="G157" s="167"/>
+      <c r="H157" s="167"/>
+      <c r="I157" s="167"/>
+      <c r="J157" s="167"/>
+      <c r="K157" s="167"/>
+      <c r="L157" s="167" t="s">
+        <v>109</v>
+      </c>
+      <c r="M157" s="167"/>
+      <c r="N157" s="167"/>
+      <c r="O157" s="167"/>
+      <c r="P157" s="167"/>
+      <c r="Q157" s="167"/>
+      <c r="R157" s="167"/>
+      <c r="S157" s="167"/>
+      <c r="T157" s="167"/>
+      <c r="U157" s="167"/>
+      <c r="V157" s="167"/>
+      <c r="W157" s="167"/>
+      <c r="X157" s="167"/>
+      <c r="Y157" s="167"/>
+      <c r="Z157" s="167"/>
+      <c r="AA157" s="167"/>
+      <c r="AB157" s="167"/>
+      <c r="AC157" s="167"/>
+      <c r="AD157" s="167"/>
+      <c r="AE157" s="167"/>
+      <c r="AF157" s="167"/>
+      <c r="AG157" s="167"/>
+      <c r="AH157" s="168" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI157" s="168"/>
+      <c r="AJ157" s="168"/>
+      <c r="AK157" s="168"/>
+      <c r="AL157" s="168"/>
+      <c r="AM157" s="168"/>
+      <c r="AN157" s="168"/>
+      <c r="AO157" s="168"/>
+      <c r="AP157" s="168"/>
+      <c r="AQ157" s="168"/>
+      <c r="AR157" s="168"/>
+      <c r="AS157" s="168"/>
       <c r="AT157" s="0"/>
       <c r="AU157" s="0"/>
       <c r="AV157" s="0"/>
@@ -16808,49 +17042,57 @@
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="17"/>
-      <c r="C158" s="0"/>
-      <c r="D158" s="0"/>
-      <c r="E158" s="0"/>
-      <c r="F158" s="0"/>
-      <c r="G158" s="0"/>
-      <c r="H158" s="0"/>
-      <c r="I158" s="0"/>
-      <c r="J158" s="0"/>
-      <c r="K158" s="0"/>
-      <c r="L158" s="0"/>
-      <c r="M158" s="0"/>
-      <c r="N158" s="0"/>
-      <c r="O158" s="0"/>
-      <c r="P158" s="0"/>
-      <c r="Q158" s="0"/>
-      <c r="R158" s="0"/>
-      <c r="S158" s="0"/>
-      <c r="T158" s="0"/>
-      <c r="U158" s="0"/>
-      <c r="V158" s="0"/>
-      <c r="W158" s="0"/>
-      <c r="X158" s="0"/>
-      <c r="Y158" s="0"/>
-      <c r="Z158" s="0"/>
-      <c r="AA158" s="0"/>
-      <c r="AB158" s="0"/>
-      <c r="AC158" s="0"/>
-      <c r="AD158" s="0"/>
-      <c r="AE158" s="0"/>
-      <c r="AF158" s="0"/>
-      <c r="AG158" s="0"/>
-      <c r="AH158" s="0"/>
-      <c r="AI158" s="0"/>
-      <c r="AJ158" s="0"/>
-      <c r="AK158" s="0"/>
-      <c r="AL158" s="0"/>
-      <c r="AM158" s="0"/>
-      <c r="AN158" s="0"/>
-      <c r="AO158" s="0"/>
-      <c r="AP158" s="0"/>
-      <c r="AQ158" s="0"/>
-      <c r="AR158" s="0"/>
-      <c r="AS158" s="0"/>
+      <c r="C158" s="169" t="n">
+        <v>1</v>
+      </c>
+      <c r="D158" s="170" t="s">
+        <v>111</v>
+      </c>
+      <c r="E158" s="171"/>
+      <c r="F158" s="171"/>
+      <c r="G158" s="172"/>
+      <c r="H158" s="172"/>
+      <c r="I158" s="172"/>
+      <c r="J158" s="172"/>
+      <c r="K158" s="173"/>
+      <c r="L158" s="174" t="s">
+        <v>112</v>
+      </c>
+      <c r="M158" s="171"/>
+      <c r="N158" s="171"/>
+      <c r="O158" s="172"/>
+      <c r="P158" s="172"/>
+      <c r="Q158" s="172"/>
+      <c r="R158" s="172"/>
+      <c r="S158" s="172"/>
+      <c r="T158" s="175"/>
+      <c r="U158" s="175"/>
+      <c r="V158" s="175"/>
+      <c r="W158" s="175"/>
+      <c r="X158" s="175"/>
+      <c r="Y158" s="175"/>
+      <c r="Z158" s="175"/>
+      <c r="AA158" s="175"/>
+      <c r="AB158" s="175"/>
+      <c r="AC158" s="175"/>
+      <c r="AD158" s="175"/>
+      <c r="AE158" s="175"/>
+      <c r="AF158" s="175"/>
+      <c r="AG158" s="176"/>
+      <c r="AH158" s="177" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI158" s="178"/>
+      <c r="AJ158" s="178"/>
+      <c r="AK158" s="178"/>
+      <c r="AL158" s="178"/>
+      <c r="AM158" s="178"/>
+      <c r="AN158" s="178"/>
+      <c r="AO158" s="178"/>
+      <c r="AP158" s="178"/>
+      <c r="AQ158" s="178"/>
+      <c r="AR158" s="178"/>
+      <c r="AS158" s="179"/>
       <c r="AT158" s="0"/>
       <c r="AU158" s="0"/>
       <c r="AV158" s="0"/>
@@ -16871,50 +17113,49 @@
     </row>
     <row r="159" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="17"/>
-      <c r="C159" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D159" s="19"/>
-      <c r="E159" s="141"/>
-      <c r="F159" s="19"/>
-      <c r="G159" s="19"/>
-      <c r="H159" s="19"/>
-      <c r="I159" s="19"/>
-      <c r="J159" s="19"/>
-      <c r="K159" s="24"/>
-      <c r="L159" s="24"/>
-      <c r="M159" s="24"/>
-      <c r="N159" s="24"/>
-      <c r="O159" s="24"/>
-      <c r="P159" s="24"/>
-      <c r="Q159" s="24"/>
-      <c r="R159" s="24"/>
-      <c r="S159" s="24"/>
-      <c r="T159" s="24"/>
-      <c r="U159" s="24"/>
-      <c r="V159" s="24"/>
-      <c r="W159" s="24"/>
-      <c r="X159" s="24"/>
-      <c r="Y159" s="24"/>
-      <c r="Z159" s="24"/>
-      <c r="AA159" s="24"/>
-      <c r="AB159" s="24"/>
-      <c r="AC159" s="24"/>
-      <c r="AD159" s="24"/>
-      <c r="AF159" s="24"/>
-      <c r="AG159" s="24"/>
-      <c r="AH159" s="24"/>
-      <c r="AI159" s="24"/>
-      <c r="AJ159" s="24"/>
-      <c r="AK159" s="24"/>
-      <c r="AL159" s="24"/>
-      <c r="AM159" s="24"/>
-      <c r="AN159" s="24"/>
-      <c r="AO159" s="24"/>
-      <c r="AP159" s="24"/>
-      <c r="AQ159" s="24"/>
-      <c r="AR159" s="24"/>
-      <c r="AS159" s="24"/>
+      <c r="C159" s="180"/>
+      <c r="D159" s="181"/>
+      <c r="E159" s="182"/>
+      <c r="F159" s="182"/>
+      <c r="G159" s="183"/>
+      <c r="H159" s="183"/>
+      <c r="I159" s="183"/>
+      <c r="J159" s="183"/>
+      <c r="K159" s="184"/>
+      <c r="L159" s="181"/>
+      <c r="M159" s="182"/>
+      <c r="N159" s="182"/>
+      <c r="O159" s="183"/>
+      <c r="P159" s="183"/>
+      <c r="Q159" s="183"/>
+      <c r="R159" s="183"/>
+      <c r="S159" s="183"/>
+      <c r="T159" s="185"/>
+      <c r="U159" s="185"/>
+      <c r="V159" s="185"/>
+      <c r="W159" s="185"/>
+      <c r="X159" s="185"/>
+      <c r="Y159" s="185"/>
+      <c r="Z159" s="185"/>
+      <c r="AA159" s="185"/>
+      <c r="AB159" s="185"/>
+      <c r="AC159" s="185"/>
+      <c r="AD159" s="185"/>
+      <c r="AE159" s="185"/>
+      <c r="AF159" s="185"/>
+      <c r="AG159" s="186"/>
+      <c r="AH159" s="187"/>
+      <c r="AI159" s="188"/>
+      <c r="AJ159" s="188"/>
+      <c r="AK159" s="188"/>
+      <c r="AL159" s="188"/>
+      <c r="AM159" s="188"/>
+      <c r="AN159" s="188"/>
+      <c r="AO159" s="188"/>
+      <c r="AP159" s="188"/>
+      <c r="AQ159" s="188"/>
+      <c r="AR159" s="188"/>
+      <c r="AS159" s="189"/>
       <c r="AT159" s="24"/>
       <c r="AU159" s="24"/>
       <c r="AV159" s="19"/>
@@ -16935,48 +17176,49 @@
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="17"/>
-      <c r="D160" s="19"/>
-      <c r="E160" s="141"/>
-      <c r="F160" s="19"/>
-      <c r="G160" s="19"/>
-      <c r="H160" s="19"/>
-      <c r="I160" s="19"/>
-      <c r="J160" s="19"/>
-      <c r="K160" s="19"/>
-      <c r="L160" s="19"/>
-      <c r="M160" s="19"/>
-      <c r="N160" s="19"/>
-      <c r="O160" s="19"/>
-      <c r="P160" s="19"/>
-      <c r="Q160" s="19"/>
-      <c r="R160" s="19"/>
-      <c r="S160" s="19"/>
-      <c r="T160" s="19"/>
-      <c r="U160" s="19"/>
-      <c r="V160" s="19"/>
-      <c r="W160" s="19"/>
-      <c r="X160" s="19"/>
-      <c r="Y160" s="19"/>
-      <c r="Z160" s="19"/>
-      <c r="AA160" s="19"/>
-      <c r="AB160" s="19"/>
-      <c r="AC160" s="19"/>
-      <c r="AD160" s="19"/>
-      <c r="AE160" s="1"/>
-      <c r="AF160" s="19"/>
-      <c r="AG160" s="19"/>
-      <c r="AH160" s="19"/>
-      <c r="AI160" s="19"/>
-      <c r="AJ160" s="19"/>
-      <c r="AK160" s="19"/>
-      <c r="AL160" s="19"/>
-      <c r="AM160" s="19"/>
-      <c r="AN160" s="19"/>
-      <c r="AO160" s="0"/>
-      <c r="AP160" s="0"/>
-      <c r="AQ160" s="0"/>
-      <c r="AR160" s="0"/>
-      <c r="AS160" s="0"/>
+      <c r="C160" s="190"/>
+      <c r="D160" s="191"/>
+      <c r="E160" s="192"/>
+      <c r="F160" s="192"/>
+      <c r="G160" s="193"/>
+      <c r="H160" s="193"/>
+      <c r="I160" s="193"/>
+      <c r="J160" s="193"/>
+      <c r="K160" s="194"/>
+      <c r="L160" s="195"/>
+      <c r="M160" s="195"/>
+      <c r="N160" s="195"/>
+      <c r="O160" s="195"/>
+      <c r="P160" s="195"/>
+      <c r="Q160" s="195"/>
+      <c r="R160" s="195"/>
+      <c r="S160" s="195"/>
+      <c r="T160" s="195"/>
+      <c r="U160" s="195"/>
+      <c r="V160" s="195"/>
+      <c r="W160" s="195"/>
+      <c r="X160" s="195"/>
+      <c r="Y160" s="195"/>
+      <c r="Z160" s="195"/>
+      <c r="AA160" s="195"/>
+      <c r="AB160" s="195"/>
+      <c r="AC160" s="195"/>
+      <c r="AD160" s="195"/>
+      <c r="AE160" s="195"/>
+      <c r="AF160" s="195"/>
+      <c r="AG160" s="195"/>
+      <c r="AH160" s="196"/>
+      <c r="AI160" s="197"/>
+      <c r="AJ160" s="197"/>
+      <c r="AK160" s="197"/>
+      <c r="AL160" s="197"/>
+      <c r="AM160" s="197"/>
+      <c r="AN160" s="197"/>
+      <c r="AO160" s="197"/>
+      <c r="AP160" s="197"/>
+      <c r="AQ160" s="197"/>
+      <c r="AR160" s="197"/>
+      <c r="AS160" s="198"/>
       <c r="AT160" s="19"/>
       <c r="AU160" s="19"/>
       <c r="AV160" s="19"/>
@@ -16984,51 +17226,49 @@
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="17"/>
-      <c r="C161" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D161" s="19"/>
-      <c r="E161" s="141"/>
-      <c r="F161" s="19"/>
-      <c r="G161" s="19"/>
-      <c r="H161" s="19"/>
-      <c r="I161" s="19"/>
-      <c r="J161" s="19"/>
-      <c r="K161" s="19"/>
-      <c r="L161" s="19"/>
-      <c r="M161" s="19"/>
-      <c r="N161" s="19"/>
-      <c r="O161" s="19"/>
-      <c r="P161" s="19"/>
-      <c r="Q161" s="19"/>
-      <c r="R161" s="19"/>
-      <c r="S161" s="19"/>
-      <c r="T161" s="19"/>
-      <c r="U161" s="19"/>
-      <c r="V161" s="19"/>
-      <c r="W161" s="19"/>
-      <c r="X161" s="19"/>
-      <c r="Y161" s="19"/>
-      <c r="Z161" s="19"/>
-      <c r="AA161" s="19"/>
-      <c r="AB161" s="19"/>
-      <c r="AC161" s="19"/>
-      <c r="AD161" s="19"/>
-      <c r="AE161" s="1"/>
-      <c r="AF161" s="19"/>
-      <c r="AG161" s="19"/>
-      <c r="AH161" s="19"/>
-      <c r="AI161" s="19"/>
-      <c r="AJ161" s="19"/>
-      <c r="AK161" s="19"/>
-      <c r="AL161" s="19"/>
-      <c r="AM161" s="19"/>
-      <c r="AN161" s="19"/>
-      <c r="AO161" s="0"/>
-      <c r="AP161" s="0"/>
-      <c r="AQ161" s="0"/>
-      <c r="AR161" s="0"/>
-      <c r="AS161" s="0"/>
+      <c r="C161" s="180"/>
+      <c r="D161" s="181"/>
+      <c r="E161" s="182"/>
+      <c r="F161" s="182"/>
+      <c r="G161" s="183"/>
+      <c r="H161" s="183"/>
+      <c r="I161" s="183"/>
+      <c r="J161" s="183"/>
+      <c r="K161" s="184"/>
+      <c r="L161" s="181"/>
+      <c r="M161" s="182"/>
+      <c r="N161" s="182"/>
+      <c r="O161" s="183"/>
+      <c r="P161" s="183"/>
+      <c r="Q161" s="183"/>
+      <c r="R161" s="183"/>
+      <c r="S161" s="183"/>
+      <c r="T161" s="185"/>
+      <c r="U161" s="185"/>
+      <c r="V161" s="185"/>
+      <c r="W161" s="185"/>
+      <c r="X161" s="185"/>
+      <c r="Y161" s="185"/>
+      <c r="Z161" s="185"/>
+      <c r="AA161" s="185"/>
+      <c r="AB161" s="185"/>
+      <c r="AC161" s="185"/>
+      <c r="AD161" s="185"/>
+      <c r="AE161" s="185"/>
+      <c r="AF161" s="185"/>
+      <c r="AG161" s="186"/>
+      <c r="AH161" s="187"/>
+      <c r="AI161" s="188"/>
+      <c r="AJ161" s="188"/>
+      <c r="AK161" s="188"/>
+      <c r="AL161" s="188"/>
+      <c r="AM161" s="188"/>
+      <c r="AN161" s="188"/>
+      <c r="AO161" s="188"/>
+      <c r="AP161" s="188"/>
+      <c r="AQ161" s="188"/>
+      <c r="AR161" s="188"/>
+      <c r="AS161" s="189"/>
       <c r="AT161" s="19"/>
       <c r="AU161" s="19"/>
       <c r="AV161" s="19"/>
@@ -17042,47 +17282,49 @@
     <row r="162" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="17"/>
       <c r="B162" s="59"/>
-      <c r="C162" s="9"/>
-      <c r="D162" s="19"/>
-      <c r="E162" s="165"/>
-      <c r="F162" s="19"/>
-      <c r="G162" s="19"/>
-      <c r="H162" s="19"/>
-      <c r="I162" s="19"/>
-      <c r="J162" s="19"/>
-      <c r="K162" s="19"/>
-      <c r="L162" s="19"/>
-      <c r="M162" s="19"/>
-      <c r="N162" s="19"/>
-      <c r="O162" s="19"/>
-      <c r="P162" s="19"/>
-      <c r="Q162" s="19"/>
-      <c r="R162" s="19"/>
-      <c r="S162" s="19"/>
-      <c r="T162" s="19"/>
-      <c r="U162" s="19"/>
-      <c r="V162" s="19"/>
-      <c r="W162" s="19"/>
-      <c r="X162" s="19"/>
-      <c r="Y162" s="19"/>
-      <c r="Z162" s="19"/>
-      <c r="AA162" s="19"/>
-      <c r="AB162" s="19"/>
-      <c r="AC162" s="19"/>
-      <c r="AD162" s="19"/>
-      <c r="AF162" s="19"/>
-      <c r="AG162" s="19"/>
-      <c r="AH162" s="19"/>
-      <c r="AI162" s="19"/>
-      <c r="AJ162" s="19"/>
-      <c r="AK162" s="19"/>
-      <c r="AL162" s="19"/>
-      <c r="AM162" s="19"/>
-      <c r="AN162" s="19"/>
-      <c r="AO162" s="0"/>
-      <c r="AP162" s="0"/>
-      <c r="AQ162" s="0"/>
-      <c r="AR162" s="0"/>
+      <c r="C162" s="190"/>
+      <c r="D162" s="191"/>
+      <c r="E162" s="192"/>
+      <c r="F162" s="192"/>
+      <c r="G162" s="193"/>
+      <c r="H162" s="193"/>
+      <c r="I162" s="193"/>
+      <c r="J162" s="193"/>
+      <c r="K162" s="194"/>
+      <c r="L162" s="195"/>
+      <c r="M162" s="195"/>
+      <c r="N162" s="195"/>
+      <c r="O162" s="195"/>
+      <c r="P162" s="195"/>
+      <c r="Q162" s="195"/>
+      <c r="R162" s="195"/>
+      <c r="S162" s="195"/>
+      <c r="T162" s="195"/>
+      <c r="U162" s="195"/>
+      <c r="V162" s="195"/>
+      <c r="W162" s="195"/>
+      <c r="X162" s="195"/>
+      <c r="Y162" s="195"/>
+      <c r="Z162" s="195"/>
+      <c r="AA162" s="195"/>
+      <c r="AB162" s="195"/>
+      <c r="AC162" s="195"/>
+      <c r="AD162" s="195"/>
+      <c r="AE162" s="195"/>
+      <c r="AF162" s="195"/>
+      <c r="AG162" s="195"/>
+      <c r="AH162" s="196"/>
+      <c r="AI162" s="197"/>
+      <c r="AJ162" s="197"/>
+      <c r="AK162" s="197"/>
+      <c r="AL162" s="197"/>
+      <c r="AM162" s="197"/>
+      <c r="AN162" s="197"/>
+      <c r="AO162" s="197"/>
+      <c r="AP162" s="197"/>
+      <c r="AQ162" s="197"/>
+      <c r="AR162" s="197"/>
+      <c r="AS162" s="198"/>
       <c r="AW162" s="20"/>
       <c r="AX162" s="99"/>
       <c r="BI162" s="0"/>
@@ -17095,14 +17337,15 @@
     <row r="163" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="0"/>
       <c r="B163" s="0"/>
-      <c r="C163" s="0" t="s">
-        <v>110</v>
-      </c>
+      <c r="C163" s="0"/>
       <c r="D163" s="0"/>
       <c r="E163" s="0"/>
       <c r="F163" s="0"/>
       <c r="G163" s="0"/>
       <c r="H163" s="0"/>
+      <c r="I163" s="0"/>
+      <c r="J163" s="0"/>
+      <c r="K163" s="0"/>
       <c r="AP163" s="19"/>
       <c r="AQ163" s="0"/>
       <c r="AR163" s="0"/>
@@ -17432,12 +17675,17 @@
     <row r="168" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0"/>
       <c r="B168" s="0"/>
-      <c r="C168" s="0"/>
-      <c r="D168" s="0"/>
-      <c r="E168" s="0"/>
-      <c r="F168" s="0"/>
-      <c r="G168" s="0"/>
-      <c r="H168" s="0"/>
+      <c r="C168" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D168" s="19"/>
+      <c r="E168" s="141"/>
+      <c r="F168" s="19"/>
+      <c r="G168" s="19"/>
+      <c r="H168" s="19"/>
+      <c r="I168" s="19"/>
+      <c r="J168" s="19"/>
+      <c r="K168" s="24"/>
       <c r="AP168" s="19"/>
       <c r="AQ168" s="0"/>
       <c r="AR168" s="0"/>
@@ -17499,12 +17747,15 @@
     <row r="169" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0"/>
       <c r="B169" s="0"/>
-      <c r="C169" s="0"/>
-      <c r="D169" s="0"/>
-      <c r="E169" s="0"/>
-      <c r="F169" s="0"/>
-      <c r="G169" s="0"/>
-      <c r="H169" s="0"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="19"/>
+      <c r="E169" s="141"/>
+      <c r="F169" s="19"/>
+      <c r="G169" s="19"/>
+      <c r="H169" s="19"/>
+      <c r="I169" s="19"/>
+      <c r="J169" s="19"/>
+      <c r="K169" s="19"/>
       <c r="AP169" s="19"/>
       <c r="AQ169" s="0"/>
       <c r="AR169" s="0"/>
@@ -17566,12 +17817,17 @@
     <row r="170" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0"/>
       <c r="B170" s="0"/>
-      <c r="C170" s="0"/>
-      <c r="D170" s="0"/>
-      <c r="E170" s="0"/>
-      <c r="F170" s="0"/>
-      <c r="G170" s="0"/>
-      <c r="H170" s="0"/>
+      <c r="C170" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D170" s="19"/>
+      <c r="E170" s="141"/>
+      <c r="F170" s="19"/>
+      <c r="G170" s="19"/>
+      <c r="H170" s="19"/>
+      <c r="I170" s="19"/>
+      <c r="J170" s="19"/>
+      <c r="K170" s="19"/>
       <c r="AP170" s="19"/>
       <c r="AQ170" s="0"/>
       <c r="AR170" s="0"/>
@@ -17633,12 +17889,15 @@
     <row r="171" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0"/>
       <c r="B171" s="0"/>
-      <c r="C171" s="0"/>
-      <c r="D171" s="0"/>
-      <c r="E171" s="0"/>
-      <c r="F171" s="0"/>
-      <c r="G171" s="0"/>
-      <c r="H171" s="0"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="19"/>
+      <c r="E171" s="165"/>
+      <c r="F171" s="19"/>
+      <c r="G171" s="19"/>
+      <c r="H171" s="19"/>
+      <c r="I171" s="19"/>
+      <c r="J171" s="19"/>
+      <c r="K171" s="19"/>
       <c r="AP171" s="19"/>
       <c r="AQ171" s="0"/>
       <c r="AR171" s="0"/>
@@ -17700,7 +17959,9 @@
     <row r="172" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0"/>
       <c r="B172" s="0"/>
-      <c r="C172" s="0"/>
+      <c r="C172" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="D172" s="0"/>
       <c r="E172" s="0"/>
       <c r="F172" s="0"/>
@@ -18233,21 +18494,56 @@
       <c r="AMI179" s="0"/>
       <c r="AMJ179" s="0"/>
     </row>
-    <row r="180" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0"/>
-      <c r="B180" s="0"/>
-      <c r="C180" s="0"/>
-      <c r="D180" s="0"/>
-      <c r="E180" s="0"/>
-      <c r="F180" s="0"/>
-      <c r="G180" s="0"/>
-      <c r="H180" s="0"/>
-      <c r="AP180" s="19"/>
-      <c r="AQ180" s="0"/>
-      <c r="AR180" s="0"/>
+    <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="26"/>
+      <c r="B180" s="26"/>
+      <c r="C180" s="26"/>
+      <c r="D180" s="26"/>
+      <c r="E180" s="26"/>
+      <c r="F180" s="26"/>
+      <c r="G180" s="26"/>
+      <c r="H180" s="26"/>
+      <c r="I180" s="26"/>
+      <c r="J180" s="26"/>
+      <c r="K180" s="26"/>
+      <c r="L180" s="26"/>
+      <c r="M180" s="26"/>
+      <c r="N180" s="26"/>
+      <c r="O180" s="26"/>
+      <c r="P180" s="26"/>
+      <c r="Q180" s="26"/>
+      <c r="R180" s="26"/>
+      <c r="S180" s="26"/>
+      <c r="T180" s="26"/>
+      <c r="U180" s="26"/>
+      <c r="V180" s="26"/>
+      <c r="W180" s="26"/>
+      <c r="X180" s="26"/>
+      <c r="Y180" s="26"/>
+      <c r="Z180" s="26"/>
+      <c r="AA180" s="26"/>
+      <c r="AB180" s="26"/>
+      <c r="AC180" s="26"/>
+      <c r="AD180" s="26"/>
+      <c r="AE180" s="26"/>
+      <c r="AF180" s="26"/>
+      <c r="AG180" s="26"/>
+      <c r="AH180" s="26"/>
+      <c r="AI180" s="26"/>
+      <c r="AJ180" s="26"/>
+      <c r="AK180" s="26"/>
+      <c r="AL180" s="26"/>
+      <c r="AM180" s="26"/>
+      <c r="AN180" s="26"/>
+      <c r="AO180" s="26"/>
+      <c r="AP180" s="26"/>
+      <c r="AQ180" s="26"/>
+      <c r="AR180" s="26"/>
+      <c r="AS180" s="26"/>
+      <c r="AT180" s="26"/>
+      <c r="AU180" s="26"/>
       <c r="AV180" s="26"/>
       <c r="AW180" s="27"/>
-      <c r="AX180" s="99"/>
       <c r="BI180" s="0"/>
       <c r="AKL180" s="0"/>
       <c r="AKM180" s="0"/>
@@ -18302,20 +18598,15 @@
       <c r="AMJ180" s="0"/>
     </row>
     <row r="181" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="25"/>
-      <c r="B181" s="166"/>
-      <c r="C181" s="26"/>
-      <c r="E181" s="167"/>
+      <c r="A181" s="9"/>
+      <c r="B181" s="59"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
       <c r="AQ181" s="0"/>
       <c r="AR181" s="0"/>
-      <c r="AS181" s="0"/>
-      <c r="AT181" s="0"/>
-      <c r="AU181" s="0"/>
-      <c r="AV181" s="0"/>
-      <c r="AW181" s="0"/>
-      <c r="AX181" s="0"/>
-      <c r="AY181" s="0"/>
-      <c r="AZ181" s="0"/>
+      <c r="AU181" s="9"/>
+      <c r="AV181" s="9"/>
       <c r="BI181" s="0"/>
     </row>
     <row r="182" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18328,23 +18619,12 @@
       <c r="AR182" s="0"/>
       <c r="AU182" s="9"/>
       <c r="AV182" s="9"/>
+      <c r="AW182" s="99"/>
       <c r="BI182" s="0"/>
     </row>
-    <row r="183" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="9"/>
-      <c r="B183" s="59"/>
-      <c r="C183" s="9"/>
-      <c r="D183" s="9"/>
-      <c r="E183" s="9"/>
-      <c r="AQ183" s="0"/>
-      <c r="AR183" s="0"/>
-      <c r="AU183" s="9"/>
-      <c r="AV183" s="9"/>
-      <c r="AW183" s="99"/>
-      <c r="BI183" s="0"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="104">
+  <mergeCells count="109">
     <mergeCell ref="A1:I3"/>
     <mergeCell ref="J1:O3"/>
     <mergeCell ref="P1:U3"/>
@@ -18449,6 +18729,11 @@
     <mergeCell ref="D148:M148"/>
     <mergeCell ref="N148:W148"/>
     <mergeCell ref="X148:AV148"/>
+    <mergeCell ref="D157:K157"/>
+    <mergeCell ref="L157:AG157"/>
+    <mergeCell ref="AH157:AS157"/>
+    <mergeCell ref="L160:AG160"/>
+    <mergeCell ref="L162:AG162"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="0.590277777777778" bottom="0.590277777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>